<commit_message>
added by user api
</commit_message>
<xml_diff>
--- a/worklogs.xlsx
+++ b/worklogs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
   <si>
     <t>WorkLogId</t>
   </si>
@@ -53,6 +53,36 @@
   </si>
   <si>
     <t>9b31bc85-ee9b-4b51-9da3-2b5f86be7e22</t>
+  </si>
+  <si>
+    <t>c14a7081-7f59-4aa1-87bb-d862ecae9fd3</t>
+  </si>
+  <si>
+    <t>c0a80cef-bb06-4186-a7fd-baaa55dde099</t>
+  </si>
+  <si>
+    <t>12f2c227-ea3c-4b63-9594-c79b33a42493</t>
+  </si>
+  <si>
+    <t>85ad201a-5ea1-461c-8278-26c0cbffd498</t>
+  </si>
+  <si>
+    <t>aea1040a-fa40-4e96-9424-9f23a1b016c7</t>
+  </si>
+  <si>
+    <t>cea04dc5-ae8c-436e-b94b-c5eaaa70580c</t>
+  </si>
+  <si>
+    <t>b7dcea3e-a338-4e45-a8ad-80833c8e17d7</t>
+  </si>
+  <si>
+    <t>3d7eeb90-8ab8-467e-a5ae-8c884b3eccf1</t>
+  </si>
+  <si>
+    <t>Sameer Butt</t>
+  </si>
+  <si>
+    <t>2fb3402f-aa9d-4692-bd3f-23b162bd27f2</t>
   </si>
 </sst>
 </file>
@@ -430,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -502,6 +532,225 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45456.74609739584</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45456.75747729167</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45457.51684482639</v>
+      </c>
+      <c r="E6" s="1">
+        <v>45457.51690163194</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
+        <v>45457.51694746528</v>
+      </c>
+      <c r="E7" s="1">
+        <v>45457.51704856481</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45457.53117403935</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45457.64254168981</v>
+      </c>
+      <c r="E9" s="1">
+        <v>45457.64597978009</v>
+      </c>
+      <c r="F9">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45457.64610547454</v>
+      </c>
+      <c r="E10" s="1">
+        <v>45457.64625344907</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45457.64976306713</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45457.66241030092</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added daily worklog sheet
</commit_message>
<xml_diff>
--- a/worklogs.xlsx
+++ b/worklogs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>WorkLogId</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>IT</t>
+  </si>
+  <si>
+    <t>06f61e43-6fc6-4ad2-8b18-68290b7dc68c</t>
+  </si>
+  <si>
+    <t>b4ee870e-ee7a-4152-b5d3-f40ee4f6bfb6</t>
+  </si>
+  <si>
+    <t>81646156-cfb4-4182-a5d0-8f76f3b681fe</t>
   </si>
 </sst>
 </file>
@@ -427,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -479,6 +488,58 @@
         <v>11</v>
       </c>
       <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>45469.50799246528</v>
+      </c>
+      <c r="E3" s="1">
+        <v>45469.50807127314</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45469.50818040509</v>
+      </c>
+      <c r="E4" s="1">
+        <v>45469.508230810185</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>